<commit_message>
My Info page is done
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/data/Source_File.xlsx
+++ b/src/main/java/org/example/data/Source_File.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148">
   <si>
     <t>Firstname</t>
   </si>
@@ -295,6 +295,12 @@
 </t>
   </si>
   <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>Editing my information</t>
+  </si>
+  <si>
     <t>S6TC001</t>
   </si>
   <si>
@@ -380,6 +386,9 @@
   </si>
   <si>
     <t>Admin page text validation</t>
+  </si>
+  <si>
+    <t>S7TC001</t>
   </si>
   <si>
     <t>User should see all the links in the Admin page</t>
@@ -398,9 +407,15 @@
 </t>
   </si>
   <si>
+    <t>S8</t>
+  </si>
+  <si>
     <t>Manage admin page</t>
   </si>
   <si>
+    <t>S8TC001</t>
+  </si>
+  <si>
     <t xml:space="preserve">User should be able to create a new system user </t>
   </si>
   <si>
@@ -428,13 +443,13 @@
     <t>User sohuld able to select "ESS"</t>
   </si>
   <si>
-    <t>Type "Paul Collings" in hte "Employee Name" textbox</t>
+    <t>Type "Mily Hm" in hte "Employee Name" textbox</t>
   </si>
   <si>
     <t>User should be able to enter the name in the "Employee Name textbox</t>
   </si>
   <si>
-    <t>type "Mily." in the username textbox</t>
+    <t>type "Mily.hm" in the username textbox</t>
   </si>
   <si>
     <t>Click "Status" label</t>
@@ -468,6 +483,9 @@
   </si>
   <si>
     <t>User should see "Mily" in hte list</t>
+  </si>
+  <si>
+    <t>S8TC002</t>
   </si>
 </sst>
 </file>
@@ -475,9 +493,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -512,8 +530,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -535,14 +576,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -551,83 +584,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -643,7 +601,67 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -664,187 +682,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,24 +873,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -906,6 +906,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -917,6 +935,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -944,168 +973,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1120,9 +1138,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1467,31 +1482,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1506,8 +1521,8 @@
   <sheetPr/>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53:D64"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -1557,10 +1572,10 @@
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1568,10 +1583,10 @@
       <c r="A3" s="4"/>
       <c r="B3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1579,10 +1594,10 @@
       <c r="A4" s="4"/>
       <c r="B4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1590,10 +1605,10 @@
       <c r="A5" s="4"/>
       <c r="B5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1601,10 +1616,10 @@
       <c r="A6" s="4"/>
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1613,10 +1628,10 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1625,10 +1640,10 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1641,10 +1656,10 @@
       <c r="D9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1653,10 +1668,10 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1665,10 +1680,10 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1677,10 +1692,10 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1697,10 +1712,10 @@
       <c r="D13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1709,10 +1724,10 @@
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1721,10 +1736,10 @@
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1733,10 +1748,10 @@
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1749,10 +1764,10 @@
       <c r="D17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1761,10 +1776,10 @@
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1773,10 +1788,10 @@
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1785,10 +1800,10 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1801,10 +1816,10 @@
       <c r="D21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1813,10 +1828,10 @@
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1825,10 +1840,10 @@
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1841,10 +1856,10 @@
       <c r="D24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1853,10 +1868,10 @@
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1865,10 +1880,10 @@
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1881,10 +1896,10 @@
       <c r="D27" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1893,10 +1908,10 @@
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1905,10 +1920,10 @@
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1921,10 +1936,10 @@
       <c r="D30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1933,10 +1948,10 @@
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1945,10 +1960,10 @@
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="5" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1957,10 +1972,10 @@
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="5" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1977,7 +1992,7 @@
       <c r="D34" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F34" s="1" t="s">
@@ -1997,7 +2012,7 @@
       <c r="D35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F35" s="1" t="s">
@@ -2017,183 +2032,190 @@
       <c r="D36" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="5" t="s">
         <v>77</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
-      <c r="B37" s="5"/>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="C37" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" ht="28" spans="2:6">
-      <c r="B38" s="5"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="6" t="s">
-        <v>88</v>
+      <c r="E38" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" ht="28" spans="2:6">
-      <c r="B39" s="5"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="6" t="s">
-        <v>90</v>
+      <c r="E39" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" ht="28" spans="2:6">
-      <c r="B40" s="5"/>
+      <c r="B40" s="2"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
-      <c r="E40" s="6" t="s">
-        <v>92</v>
+      <c r="E40" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" ht="28" spans="2:6">
-      <c r="B41" s="5"/>
+      <c r="B41" s="2"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="6" t="s">
-        <v>94</v>
+      <c r="E41" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" ht="28" spans="2:6">
-      <c r="B42" s="5"/>
+      <c r="B42" s="2"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="6" t="s">
-        <v>96</v>
+      <c r="E42" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="2:6">
-      <c r="B43" s="5"/>
+      <c r="B43" s="2"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-      <c r="E43" s="6" t="s">
-        <v>98</v>
+      <c r="E43" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="2:6">
-      <c r="B44" s="5"/>
+      <c r="B44" s="2"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
-      <c r="E44" s="6" t="s">
-        <v>100</v>
+      <c r="E44" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="2:6">
-      <c r="B45" s="5"/>
+      <c r="B45" s="2"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="6" t="s">
-        <v>102</v>
+      <c r="E45" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="2:6">
-      <c r="B46" s="5"/>
+      <c r="B46" s="2"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-      <c r="E46" s="6" t="s">
-        <v>104</v>
+      <c r="E46" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="2:6">
-      <c r="B47" s="5"/>
+      <c r="B47" s="2"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
-      <c r="E47" s="6" t="s">
-        <v>106</v>
+      <c r="E47" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="2:6">
-      <c r="B48" s="5"/>
+      <c r="B48" s="2"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-      <c r="E48" s="6" t="s">
-        <v>108</v>
+      <c r="E48" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="2:6">
-      <c r="B49" s="5"/>
+      <c r="B49" s="2"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-      <c r="E49" s="6" t="s">
-        <v>104</v>
+      <c r="E49" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="5"/>
+      <c r="B50" s="2"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="6"/>
+      <c r="E50" s="5"/>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C51" s="4"/>
+        <v>114</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D51" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F51" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" ht="56" spans="2:6">
@@ -2201,25 +2223,30 @@
       <c r="C52" s="4"/>
       <c r="D52" s="2"/>
       <c r="E52" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="B53" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" s="4"/>
+        <v>122</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="D53" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E53" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="2:6">
@@ -2227,10 +2254,10 @@
       <c r="C54" s="4"/>
       <c r="D54" s="2"/>
       <c r="E54" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" ht="28" spans="2:6">
@@ -2238,10 +2265,10 @@
       <c r="C55" s="4"/>
       <c r="D55" s="2"/>
       <c r="E55" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="2:6">
@@ -2249,10 +2276,10 @@
       <c r="C56" s="4"/>
       <c r="D56" s="2"/>
       <c r="E56" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" ht="28" spans="2:6">
@@ -2260,10 +2287,10 @@
       <c r="C57" s="4"/>
       <c r="D57" s="2"/>
       <c r="E57" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="2:6">
@@ -2271,7 +2298,7 @@
       <c r="C58" s="4"/>
       <c r="D58" s="2"/>
       <c r="E58" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>23</v>
@@ -2282,10 +2309,10 @@
       <c r="C59" s="4"/>
       <c r="D59" s="2"/>
       <c r="E59" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="2:6">
@@ -2293,10 +2320,10 @@
       <c r="C60" s="4"/>
       <c r="D60" s="2"/>
       <c r="E60" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F60" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" ht="28" spans="2:6">
@@ -2304,10 +2331,10 @@
       <c r="C61" s="4"/>
       <c r="D61" s="2"/>
       <c r="E61" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" ht="28" spans="2:6">
@@ -2315,10 +2342,10 @@
       <c r="C62" s="4"/>
       <c r="D62" s="2"/>
       <c r="E62" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="2:6">
@@ -2326,10 +2353,10 @@
       <c r="C63" s="4"/>
       <c r="D63" s="2"/>
       <c r="E63" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="2:6">
@@ -2337,22 +2364,25 @@
       <c r="C64" s="4"/>
       <c r="D64" s="2"/>
       <c r="E64" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F64" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="8"/>
+      <c r="C65" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D65" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="A13:A33"/>
+    <mergeCell ref="A37:A50"/>
     <mergeCell ref="A51:A52"/>
     <mergeCell ref="A53:A64"/>
     <mergeCell ref="B2:B12"/>

</xml_diff>

<commit_message>
My Info Page Done
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/data/Source_File.xlsx
+++ b/src/main/java/org/example/data/Source_File.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173">
   <si>
     <t>Firstname</t>
   </si>
@@ -107,13 +107,13 @@
     <t>Popup should be closed, user should land on "Dashboard" tab</t>
   </si>
   <si>
-    <t>click "Welcome Paul" link at the right top corener of the page</t>
+    <t>Click "Welcome Paul" link at the right top corener of the page</t>
   </si>
   <si>
     <t>"About" and "Logout" options should be available in the dropdown</t>
   </si>
   <si>
-    <t>click "Logout" button</t>
+    <t>Click "Logout" button</t>
   </si>
   <si>
     <t>User should land on login page and the Orange HRM website logo should be seen</t>
@@ -125,19 +125,19 @@
     <t>User should see success message when putting the valid username while resetting the password</t>
   </si>
   <si>
-    <t>click "Forgot your password?" link</t>
+    <t>Click "Forgot your password?" link</t>
   </si>
   <si>
     <t>User should see Orange HRM website logo, and header "Forgot Your Password?", text "Please enter your username to identify your account to reset your password."</t>
   </si>
   <si>
-    <t>input valid username into "OrangeHRM Username" input box</t>
+    <t>Input valid username into "OrangeHRM Username" input box</t>
   </si>
   <si>
     <t>User should be able to input valid username</t>
   </si>
   <si>
-    <t>click "Reset Password" button</t>
+    <t>Click "Reset Password" button</t>
   </si>
   <si>
     <t>User should see header "Instruction Sent !",
@@ -213,7 +213,7 @@
     <t>User should reveive error message when inputting special characters/ WRONG usernme in the "OrangeHRM Username" input box while resetting the password</t>
   </si>
   <si>
-    <t xml:space="preserve">input special characters in the "OrangeHRM Username" input box </t>
+    <t xml:space="preserve">Input special characters in the "OrangeHRM Username" input box </t>
   </si>
   <si>
     <t>User should be able to enter special characters</t>
@@ -307,7 +307,7 @@
     <t>User should be able to edit personal information</t>
   </si>
   <si>
-    <t>navigate to MyInfo Page</t>
+    <t>Navigate to MyInfo Page</t>
   </si>
   <si>
     <t xml:space="preserve">User should see MyInfo Page </t>
@@ -319,22 +319,22 @@
     <t>User should be able to click "Edit" button</t>
   </si>
   <si>
-    <t>type "Mily" in the firstname inputbox</t>
-  </si>
-  <si>
-    <t>User shuold be able to type "Mily" in the inputbox</t>
-  </si>
-  <si>
-    <t>type "Hm" in the lastname inputbox</t>
-  </si>
-  <si>
-    <t>User should be able to type "Hm" in the inputbox</t>
-  </si>
-  <si>
-    <t>Type"007" in the "Employee ID" inputbox</t>
-  </si>
-  <si>
-    <t>User should be able to Type"007" in the "Employee ID" inputbox</t>
+    <t>Enter "Mily" in the firstname inputbox</t>
+  </si>
+  <si>
+    <t>User shuold be able to enter "Mily" in the inputbox</t>
+  </si>
+  <si>
+    <t>Enter "Hm" in the lastname inputbox</t>
+  </si>
+  <si>
+    <t>User should be able to enter "Hm" in the inputbox</t>
+  </si>
+  <si>
+    <t>Enter "007" in the "Employee ID" inputbox</t>
+  </si>
+  <si>
+    <t>User should be able to enter "007" in the "Employee ID" inputbox</t>
   </si>
   <si>
     <t>Select"2023-09-01" from the "License Expiry Date" list</t>
@@ -343,7 +343,7 @@
     <t xml:space="preserve">User should be able to select"2023-09-01" in the "License Expiry Date" </t>
   </si>
   <si>
-    <t xml:space="preserve">click "Female" radioButton in "Gender " </t>
+    <t xml:space="preserve">Click "Female" radioButton in "Gender " </t>
   </si>
   <si>
     <t>User should be able to click "Female"</t>
@@ -394,10 +394,10 @@
     <t>User should be to click "choose file" button</t>
   </si>
   <si>
-    <t>Type file path</t>
-  </si>
-  <si>
-    <t>User should be able to type file path</t>
+    <t>Enter file path</t>
+  </si>
+  <si>
+    <t>User should be able to enter file path</t>
   </si>
   <si>
     <t>Click on "upload" button</t>
@@ -433,10 +433,10 @@
     <t xml:space="preserve">User should see Admin link </t>
   </si>
   <si>
-    <t>click "Admin" link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user should see following links: "User Management","Job","Organization","Qualifications","Nationalities","Configuration";
+    <t>Click "Admin" link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see following links: "User Management","Job","Organization","Qualifications","Nationalities","Configuration";
 </t>
   </si>
   <si>
@@ -452,16 +452,16 @@
     <t>User should be able to add a new system user to the admin page</t>
   </si>
   <si>
-    <t>navigate to admin Page</t>
+    <t>Navigate to admin Page</t>
   </si>
   <si>
     <t>User should see Admin Page</t>
   </si>
   <si>
-    <t>click "Add" button</t>
-  </si>
-  <si>
-    <t>click "User Role" label</t>
+    <t>Click "Add" button</t>
+  </si>
+  <si>
+    <t>Click "User Role" label</t>
   </si>
   <si>
     <t>User sohuld see All", "Admin","ESS" in "User Role" label</t>
@@ -473,13 +473,13 @@
     <t>User sohuld able to select "ESS"</t>
   </si>
   <si>
-    <t>Type "Mily Hm" in hte "Employee Name" textbox</t>
+    <t>Enter "Mily Hm" in hte "Employee Name" textbox</t>
   </si>
   <si>
     <t>User should be able to enter the name in the "Employee Name textbox</t>
   </si>
   <si>
-    <t>type "Mily." in the username textbox</t>
+    <t>Enter "Mily." in the username textbox</t>
   </si>
   <si>
     <t>Click "Status" label</t>
@@ -494,7 +494,7 @@
     <t>User should be able to click "Enable" button</t>
   </si>
   <si>
-    <t>enter "Mily1234" in the password textbox</t>
+    <t>Enter "Mily1234" in the password textbox</t>
   </si>
   <si>
     <t>User should be able to enter "Mily1234" in the password textbox</t>
@@ -506,10 +506,10 @@
     <t>User should be able to Reenter "Mily1234" in the confirm password textbox</t>
   </si>
   <si>
-    <t>click save button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verify "Mily" display in the list </t>
+    <t>Click save button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify "Mily" display in the list </t>
   </si>
   <si>
     <t>User should see "Mily" in hte list</t>
@@ -524,28 +524,43 @@
     <t>S9TC001</t>
   </si>
   <si>
-    <t>User should be able to seach a system user from the admin page</t>
+    <t>User should be able to seach a system user from admin page</t>
   </si>
   <si>
     <t>User should see admin page</t>
   </si>
   <si>
-    <t>type "Milyyy"in the "username" textField</t>
-  </si>
-  <si>
-    <t>User should be able to type username</t>
-  </si>
-  <si>
-    <t>click on "Search" button</t>
+    <t>Enter "Milyyy"in the "username" textField</t>
+  </si>
+  <si>
+    <t>User should be able to enter username</t>
+  </si>
+  <si>
+    <t>Click on "Search" button</t>
   </si>
   <si>
     <t>User should be able to click "search" button</t>
   </si>
   <si>
-    <t>verify "Milyyy" record display</t>
+    <t>Verify "Milyyy" record display</t>
   </si>
   <si>
     <t>User should see "Milyyy" on the resut list</t>
+  </si>
+  <si>
+    <t>S9TC002</t>
+  </si>
+  <si>
+    <t>User should be able to seach an invalid system user from admin page</t>
+  </si>
+  <si>
+    <t>Enter "Alex.X"in the "username" textField</t>
+  </si>
+  <si>
+    <t>Verify "No Records Found" message display</t>
+  </si>
+  <si>
+    <t>User should see"No Records Found" messge</t>
   </si>
 </sst>
 </file>
@@ -553,9 +568,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -584,15 +599,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -606,8 +613,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -621,16 +636,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -638,22 +646,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -676,7 +668,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -689,9 +696,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -705,7 +712,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -720,8 +727,16 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -742,187 +757,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,21 +948,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -975,13 +975,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -997,6 +1001,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1019,16 +1034,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1038,152 +1053,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1204,6 +1219,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1542,31 +1560,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1581,8 +1599,8 @@
   <sheetPr/>
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -2499,7 +2517,7 @@
       <c r="C70" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="4" t="s">
         <v>160</v>
       </c>
       <c r="E70" t="s">
@@ -2512,7 +2530,7 @@
     <row r="71" spans="2:6">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="2"/>
+      <c r="D71" s="4"/>
       <c r="E71" t="s">
         <v>162</v>
       </c>
@@ -2523,7 +2541,7 @@
     <row r="72" spans="2:6">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
-      <c r="D72" s="2"/>
+      <c r="D72" s="4"/>
       <c r="E72" t="s">
         <v>164</v>
       </c>
@@ -2534,7 +2552,7 @@
     <row r="73" spans="2:6">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="2"/>
+      <c r="D73" s="4"/>
       <c r="E73" t="s">
         <v>166</v>
       </c>
@@ -2542,47 +2560,83 @@
         <v>167</v>
       </c>
     </row>
-    <row r="74" spans="2:2">
-      <c r="B74" s="7"/>
-    </row>
-    <row r="75" spans="2:2">
-      <c r="B75" s="7"/>
-    </row>
-    <row r="76" spans="2:2">
-      <c r="B76" s="7"/>
-    </row>
-    <row r="77" spans="2:2">
-      <c r="B77" s="7"/>
+    <row r="74" spans="2:6">
+      <c r="B74" s="4"/>
+      <c r="C74" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E74" t="s">
+        <v>128</v>
+      </c>
+      <c r="F74" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" s="4"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="7"/>
+      <c r="E75" t="s">
+        <v>170</v>
+      </c>
+      <c r="F75" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6">
+      <c r="B76" s="4"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="7"/>
+      <c r="E76" t="s">
+        <v>164</v>
+      </c>
+      <c r="F76" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="B77" s="4"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="7"/>
+      <c r="E77" t="s">
+        <v>171</v>
+      </c>
+      <c r="F77" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="7"/>
+      <c r="B78" s="8"/>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="7"/>
+      <c r="B79" s="8"/>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="7"/>
+      <c r="B80" s="8"/>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="7"/>
+      <c r="B81" s="8"/>
     </row>
     <row r="82" spans="2:2">
       <c r="B82" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="38">
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="A13:A33"/>
     <mergeCell ref="A37:A55"/>
     <mergeCell ref="A56:A57"/>
     <mergeCell ref="A58:A69"/>
-    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A70:A77"/>
     <mergeCell ref="B2:B12"/>
     <mergeCell ref="B13:B33"/>
     <mergeCell ref="B37:B55"/>
     <mergeCell ref="B56:B57"/>
     <mergeCell ref="B58:B69"/>
-    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B70:B77"/>
     <mergeCell ref="C2:C8"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="C13:C16"/>
@@ -2595,6 +2649,7 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="C58:C69"/>
     <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C74:C77"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="D9:D12"/>
     <mergeCell ref="D13:D16"/>
@@ -2607,6 +2662,7 @@
     <mergeCell ref="D56:D57"/>
     <mergeCell ref="D58:D69"/>
     <mergeCell ref="D70:D73"/>
+    <mergeCell ref="D74:D77"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Admin page, Dashboard page, PIM page, Leave Page are done.
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/data/Source_File.xlsx
+++ b/src/main/java/org/example/data/Source_File.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11780" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373">
   <si>
     <t>Firstname</t>
   </si>
@@ -298,7 +298,7 @@
     <t>S6</t>
   </si>
   <si>
-    <t>Editing My information Page</t>
+    <t>Editing personal information</t>
   </si>
   <si>
     <t>S6TC001</t>
@@ -418,19 +418,295 @@
     <t>S7</t>
   </si>
   <si>
+    <t xml:space="preserve">Updating contact details </t>
+  </si>
+  <si>
+    <t>S7TC001</t>
+  </si>
+  <si>
+    <t>User should be able to update contact details</t>
+  </si>
+  <si>
+    <t>Click "My Info" link</t>
+  </si>
+  <si>
+    <t>User should be able to click "My Info" link</t>
+  </si>
+  <si>
+    <t>Click "Contact Details" button</t>
+  </si>
+  <si>
+    <t>User should be able to click "Contact Details" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on "Edit" button </t>
+  </si>
+  <si>
+    <t>User should be able to click "Edit" ubtton</t>
+  </si>
+  <si>
+    <t>Enter"456 Morris Drive" in "in Address Street 1" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter"456 Morris Drive" in "in Address Street 1" input field</t>
+  </si>
+  <si>
+    <t>Enter"apt 101" in "in Address Street 2" input field</t>
+  </si>
+  <si>
+    <t>user should be able to enter"apt 101" in "in Address Street 2" input field</t>
+  </si>
+  <si>
+    <t>Enter "Anchorage" in City inpur field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "Anchorage" in City inpur field</t>
+  </si>
+  <si>
+    <t>Enter "Alaska" in "State/Province" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "Alaska" in "State/Province" input field</t>
+  </si>
+  <si>
+    <t>Enter "12340" in "Zip/Postal Cod" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "12340" in "Zip/Postal Cod" input field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select "United states" in "Country" dropdown list </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to select "united states" </t>
+  </si>
+  <si>
+    <t>Click "save" button</t>
+  </si>
+  <si>
+    <t>Verify "successfully saved" message display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see ""successfully saved" message </t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>Editing emergency contact information</t>
+  </si>
+  <si>
+    <t>S8TC001</t>
+  </si>
+  <si>
+    <t>User should be able to edit emergency contact information</t>
+  </si>
+  <si>
+    <t>Click "Emergency Contacts" button</t>
+  </si>
+  <si>
+    <t>User should be able to click "Emergency Contacts" button</t>
+  </si>
+  <si>
+    <t>Click "Add" button</t>
+  </si>
+  <si>
+    <t>User sohuld be able to click "Add" button</t>
+  </si>
+  <si>
+    <t>Enter "Daniel" in the "name" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "Daniel" in the "name" input field</t>
+  </si>
+  <si>
+    <t>Enter "Family Member" in the "Relationship" input field</t>
+  </si>
+  <si>
+    <t>User sohuld be able to enter "Family Member" in the "Relationship" input field</t>
+  </si>
+  <si>
+    <t>Enter "1234567" in "Home Telephone" input field</t>
+  </si>
+  <si>
+    <t>User sohuld be able to enter "1234567" in "Home Telephone" input field</t>
+  </si>
+  <si>
+    <t>User should be to click "save" button</t>
+  </si>
+  <si>
+    <t>Verify "Emergency Contact" information is updated</t>
+  </si>
+  <si>
+    <t>User should see updated information</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding dependents to the page </t>
+  </si>
+  <si>
+    <t>S9TC001</t>
+  </si>
+  <si>
+    <t>User should be able to add dependents to the page</t>
+  </si>
+  <si>
+    <t>Click on "My Info" link</t>
+  </si>
+  <si>
+    <t>Click "Dependents" button</t>
+  </si>
+  <si>
+    <t>User should be able to click "Dependents" button</t>
+  </si>
+  <si>
+    <t>Enter "Mike" in name input field</t>
+  </si>
+  <si>
+    <t>user should be able to enter "Mike" in name input field</t>
+  </si>
+  <si>
+    <t>Select "Child" in relationship dropdown list</t>
+  </si>
+  <si>
+    <t>User should be able to select "Child" in dropdown list</t>
+  </si>
+  <si>
+    <t>Enter"2010/01/01" in date of birth input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "2020/01/01" in date of birth iput field</t>
+  </si>
+  <si>
+    <t>Click in "save" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify "Mike' is added to the page </t>
+  </si>
+  <si>
+    <t>User should see "Mike" on the list</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>Adding immigration record to myInfo page</t>
+  </si>
+  <si>
+    <t>S10TC001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to add immigration record </t>
+  </si>
+  <si>
+    <t>Click "Immigration" link</t>
+  </si>
+  <si>
+    <t>User should be able to click "Immigration" link</t>
+  </si>
+  <si>
+    <t>Click "VIsa" radio button</t>
+  </si>
+  <si>
+    <t>User should be able to click "Visa" radio button</t>
+  </si>
+  <si>
+    <t>Enter "123456789" in number input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter"12356789" in input field</t>
+  </si>
+  <si>
+    <t>Enter "2018-04-04" in "Issued Date" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "2018-04-04"</t>
+  </si>
+  <si>
+    <t>Enter "2026-04-04" in "Expiry Date" input field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to enter "2026-04-04" </t>
+  </si>
+  <si>
+    <t>Enter "/" in "Eligible Status" input field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to enter "/" </t>
+  </si>
+  <si>
+    <t>Select "China" in "Issued By" dropdown list</t>
+  </si>
+  <si>
+    <t>User should be able to select "China"</t>
+  </si>
+  <si>
+    <t>Enter "2021-04-02" in "Eligible Review Date" input field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to enter "2021-04-02" </t>
+  </si>
+  <si>
+    <t>Enter "record added" in "Comments" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "record added" in "Comments" input field</t>
+  </si>
+  <si>
+    <t>Click "Save" button</t>
+  </si>
+  <si>
+    <t>User should be able to click "Save" button</t>
+  </si>
+  <si>
+    <t>Verify record is added to the page</t>
+  </si>
+  <si>
+    <t>User should see one record added</t>
+  </si>
+  <si>
+    <t>Deleting immigration record from myInfo page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to delete immigration record </t>
+  </si>
+  <si>
+    <t>Click the dadio button on the first row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to click the radio button </t>
+  </si>
+  <si>
+    <t>Click "Delete" button</t>
+  </si>
+  <si>
+    <t>User should see row got deleted</t>
+  </si>
+  <si>
+    <t>Verify record got deleted</t>
+  </si>
+  <si>
+    <t>User should see record got deleted</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
     <t>Admin page text validation</t>
   </si>
   <si>
-    <t>S7TC001</t>
-  </si>
-  <si>
-    <t>User should see all the links in the Admin page</t>
+    <t>S11TC001</t>
+  </si>
+  <si>
+    <t>User should see all the links on the Admin page</t>
   </si>
   <si>
     <t>Navigate to Admin Page</t>
   </si>
   <si>
-    <t xml:space="preserve">User should see Admin link </t>
+    <t>User should see Admin page</t>
   </si>
   <si>
     <t>Click "Admin" link</t>
@@ -440,13 +716,13 @@
 </t>
   </si>
   <si>
-    <t>S8</t>
-  </si>
-  <si>
-    <t>Adding new user to the page</t>
-  </si>
-  <si>
-    <t>S8TC001</t>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>Adding new user to the admin page</t>
+  </si>
+  <si>
+    <t>S12TC001</t>
   </si>
   <si>
     <t>User should be able to add a new system user to the admin page</t>
@@ -458,9 +734,6 @@
     <t>User should see Admin Page</t>
   </si>
   <si>
-    <t>Click "Add" button</t>
-  </si>
-  <si>
     <t>Click "User Role" label</t>
   </si>
   <si>
@@ -515,13 +788,13 @@
     <t>User should see "Mily" in hte list</t>
   </si>
   <si>
-    <t>S9</t>
-  </si>
-  <si>
-    <t>Searching an user from the page</t>
-  </si>
-  <si>
-    <t>S9TC001</t>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>Searching an user on the admin page</t>
+  </si>
+  <si>
+    <t>S13TC001</t>
   </si>
   <si>
     <t>User should be able to seach a system user from admin page</t>
@@ -548,10 +821,10 @@
     <t>User should see "Milyyy" on the resut list</t>
   </si>
   <si>
-    <t>S9TC002</t>
-  </si>
-  <si>
-    <t>User should be able to seach an invalid system user from admin page</t>
+    <t>S13TC002</t>
+  </si>
+  <si>
+    <t>User should see" No records found" message when seaching an invalid system user from admin page</t>
   </si>
   <si>
     <t>Enter "Alex.X"in the "username" textField</t>
@@ -561,6 +834,335 @@
   </si>
   <si>
     <t>User should see"No Records Found" messge</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding job title to the admin page </t>
+  </si>
+  <si>
+    <t>S14TC001</t>
+  </si>
+  <si>
+    <t>User should be able to add a job title to the job title list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on admin link </t>
+  </si>
+  <si>
+    <t>Click "Job" link</t>
+  </si>
+  <si>
+    <t>User should be to click "Job" link</t>
+  </si>
+  <si>
+    <t>Click "Job TItle" link</t>
+  </si>
+  <si>
+    <t>User should be able to click "Job Title" link</t>
+  </si>
+  <si>
+    <t>Enter "Businiss Manager" in job title input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "Business Manager"</t>
+  </si>
+  <si>
+    <t>Enter "plan and promote the daily schedule of employees and the business, interview, hire, and coordinate employees" in job description input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "plan and promote the daily schedule of employees and the business, interview, hire, and coordinate employees"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify job title added to the list </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see job title in the list </t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>Deleting job title form admin page</t>
+  </si>
+  <si>
+    <t>S15TC001</t>
+  </si>
+  <si>
+    <t>User should be able to delete a job tilte from admin page</t>
+  </si>
+  <si>
+    <t>User should be able to click admin link</t>
+  </si>
+  <si>
+    <t>Click on " job" link</t>
+  </si>
+  <si>
+    <t>User sohuld be able to click "job" link</t>
+  </si>
+  <si>
+    <t>CLick "Job Titles" link</t>
+  </si>
+  <si>
+    <t>User sohuld be able to click "Job TItles" link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLick on "Business Manager" checkbox </t>
+  </si>
+  <si>
+    <t>User sohuld be able to click the checkbox</t>
+  </si>
+  <si>
+    <t>Click on "Delete" button</t>
+  </si>
+  <si>
+    <t>User should be able to click "Delete" button</t>
+  </si>
+  <si>
+    <t>Click on " Ok" button</t>
+  </si>
+  <si>
+    <t>User should be able to click "Ok" button</t>
+  </si>
+  <si>
+    <t>Verfy "Business Manager" geo deleted</t>
+  </si>
+  <si>
+    <t>User should see "Business Manager" is removed on the list</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>PIM page text validation</t>
+  </si>
+  <si>
+    <t>S16TC001</t>
+  </si>
+  <si>
+    <t>User should see all the links on the PIM page</t>
+  </si>
+  <si>
+    <t>Navigate to PIM page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see PIM page </t>
+  </si>
+  <si>
+    <t>Click "PIM" link</t>
+  </si>
+  <si>
+    <t>User should see following links:Configuration, Optional Fields, Custom Fields, Data Import, Reporting Methods, Termination Reasons, Employee List, Add Employee, Reports</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>Adding new employee to the PIM page</t>
+  </si>
+  <si>
+    <t>S17TC001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to add new employee to the list </t>
+  </si>
+  <si>
+    <t>Click on PIM link</t>
+  </si>
+  <si>
+    <t>User should be able to click PIM link</t>
+  </si>
+  <si>
+    <t>Click "Add Employee" link</t>
+  </si>
+  <si>
+    <t>User should be able to click "Add Employee" link</t>
+  </si>
+  <si>
+    <t>Enter  "Pete" in "First Name" input field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to enter "Pete" </t>
+  </si>
+  <si>
+    <t>Enter "Damian" in "Last Name" input field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to enter "Damian" </t>
+  </si>
+  <si>
+    <t>Verify new employee added to the list</t>
+  </si>
+  <si>
+    <t>User shoud see new employee added to the list</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>Searching an employee on the PIM page</t>
+  </si>
+  <si>
+    <t>S18TC001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to search an employee on PIM page </t>
+  </si>
+  <si>
+    <t>Click PIM link</t>
+  </si>
+  <si>
+    <t>Enter " Pete Damian" in "Employee Name" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "Pete Damian"</t>
+  </si>
+  <si>
+    <t>Click "Search" button</t>
+  </si>
+  <si>
+    <t>Verfiy "Pete Damian" display on the page</t>
+  </si>
+  <si>
+    <t>User should see "Pete Damian" on the page</t>
+  </si>
+  <si>
+    <t>S19</t>
+  </si>
+  <si>
+    <t>Validating all the links on the leave page</t>
+  </si>
+  <si>
+    <t>S19TC001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User shuold be able to see all the links on the leave page
+</t>
+  </si>
+  <si>
+    <t>Navigate to the "Leave" page</t>
+  </si>
+  <si>
+    <t>User should see "Leave" page</t>
+  </si>
+  <si>
+    <t>Click "Leave" link</t>
+  </si>
+  <si>
+    <t>User should be able to click "Leave" link</t>
+  </si>
+  <si>
+    <t>Verify links on the "Leave" page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see following links: Apply, My Leave, Entitlements, Reports, Configure, Leave List, Assign Leave. 
+</t>
+  </si>
+  <si>
+    <t>S20</t>
+  </si>
+  <si>
+    <t>Adding a new leave list to the leave page</t>
+  </si>
+  <si>
+    <t>S20TC001</t>
+  </si>
+  <si>
+    <t>User should be able to add new leave to the page</t>
+  </si>
+  <si>
+    <t>Click "Assign Leave" link</t>
+  </si>
+  <si>
+    <t>User should be able to click "Assign Leave" link</t>
+  </si>
+  <si>
+    <t>Enter "Mily Hm" in the "Employee Name" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "Mily Hm" in the input field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select "US-Vacation" from dropdown list </t>
+  </si>
+  <si>
+    <t>User should be able to select "US-vacation"</t>
+  </si>
+  <si>
+    <t>Enter "2021-01-22" in the "From Date" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "2021-01-22"</t>
+  </si>
+  <si>
+    <t>Enter "2021-01-24" in the "To Date" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter 2021-01-24</t>
+  </si>
+  <si>
+    <t>Click "Assign" button</t>
+  </si>
+  <si>
+    <t>User should be able to click "Assign" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verfiy leave assigned to the page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see leave is assigned to the page </t>
+  </si>
+  <si>
+    <t>S21</t>
+  </si>
+  <si>
+    <t>Searching a leave list from leave page</t>
+  </si>
+  <si>
+    <t>S21TC001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to search leave list from list page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see Leave page </t>
+  </si>
+  <si>
+    <t>User should be able to click leave link</t>
+  </si>
+  <si>
+    <t>Click "Leave List" link</t>
+  </si>
+  <si>
+    <t>User should be able to click leave list link</t>
+  </si>
+  <si>
+    <t>Enter "2021-01-22" in the "From" input field</t>
+  </si>
+  <si>
+    <t>User should be able to enter "2021-01-24"</t>
+  </si>
+  <si>
+    <t>Check "All" button on "Show Leave with Status"</t>
+  </si>
+  <si>
+    <t>User should be able to check "All" checkbox button</t>
+  </si>
+  <si>
+    <t>Select "Human Resources" in "Sub Unit" dropdown list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to select "Human Resources" </t>
+  </si>
+  <si>
+    <t>User should be able to "Seatch" button</t>
+  </si>
+  <si>
+    <t>Verify search result is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see a leave list display on the page </t>
   </si>
 </sst>
 </file>
@@ -568,9 +1170,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -605,45 +1207,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -653,37 +1216,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -698,7 +1231,53 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -726,8 +1305,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -739,6 +1326,21 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -757,7 +1359,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -769,109 +1515,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -883,61 +1539,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,15 +1550,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -975,32 +1568,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1025,11 +1597,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1053,152 +1655,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1224,7 +1826,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -1560,31 +2165,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1597,10 +2202,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -2339,304 +2944,1509 @@
       <c r="A56" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F57" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="57" ht="56" spans="2:6">
-      <c r="B57" s="2"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="2"/>
-      <c r="E57" t="s">
+    <row r="58" ht="28" spans="2:6">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="E58" t="s">
-        <v>136</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="59" spans="2:6">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-      <c r="E59" t="s">
-        <v>138</v>
+      <c r="E59" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" ht="28" spans="2:6">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
-      <c r="E60" t="s">
-        <v>139</v>
+      <c r="E60" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" ht="28" spans="2:6">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
-      <c r="E61" t="s">
-        <v>141</v>
+      <c r="E61" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" ht="28" spans="2:6">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
-      <c r="E62" t="s">
-        <v>143</v>
+      <c r="E62" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" ht="28" spans="2:6">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
-      <c r="E63" t="s">
-        <v>145</v>
+      <c r="E63" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" ht="28" spans="2:6">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
-      <c r="E64" t="s">
-        <v>146</v>
+      <c r="E64" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="2:6">
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
-      <c r="E65" t="s">
-        <v>148</v>
-      </c>
-      <c r="F65" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="66" ht="28" spans="2:6">
+      <c r="E65" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
-      <c r="E66" t="s">
-        <v>150</v>
+      <c r="E66" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="67" ht="28" spans="2:6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6">
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
-      <c r="E67" t="s">
+      <c r="E67" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6">
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
       <c r="E68" t="s">
-        <v>154</v>
+        <v>88</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="2:6">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
+      <c r="D69" s="2"/>
       <c r="E69" t="s">
-        <v>155</v>
-      </c>
-      <c r="F69" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>160</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" ht="28" spans="2:6">
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="2"/>
       <c r="E70" t="s">
-        <v>128</v>
-      </c>
-      <c r="F70" t="s">
-        <v>161</v>
+        <v>153</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="2:6">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
+      <c r="D71" s="2"/>
       <c r="E71" t="s">
-        <v>162</v>
-      </c>
-      <c r="F71" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6">
+        <v>155</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" ht="28" spans="2:6">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
+      <c r="D72" s="2"/>
       <c r="E72" t="s">
-        <v>164</v>
-      </c>
-      <c r="F72" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6">
+        <v>157</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="73" ht="28" spans="2:6">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
+      <c r="D73" s="2"/>
       <c r="E73" t="s">
-        <v>166</v>
-      </c>
-      <c r="F73" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6">
+        <v>159</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" ht="28" spans="2:6">
       <c r="B74" s="4"/>
-      <c r="C74" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>169</v>
-      </c>
+      <c r="C74" s="4"/>
+      <c r="D74" s="2"/>
       <c r="E74" t="s">
-        <v>128</v>
-      </c>
-      <c r="F74" t="s">
-        <v>137</v>
+        <v>161</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="2:6">
       <c r="B75" s="4"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="7"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="2"/>
       <c r="E75" t="s">
-        <v>170</v>
-      </c>
-      <c r="F75" t="s">
+        <v>146</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="76" spans="2:6">
       <c r="B76" s="4"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="7"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="2"/>
       <c r="E76" t="s">
         <v>164</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="77" spans="2:6">
-      <c r="B77" s="4"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="7"/>
+    <row r="77" spans="1:6">
+      <c r="A77" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="E77" t="s">
+        <v>88</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="2"/>
+      <c r="E78" t="s">
+        <v>170</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="79" ht="28" spans="2:6">
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="2"/>
+      <c r="E79" t="s">
         <v>171</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F79" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="2:2">
-      <c r="B78" s="8"/>
-    </row>
-    <row r="79" spans="2:2">
-      <c r="B79" s="8"/>
-    </row>
-    <row r="80" spans="2:2">
-      <c r="B80" s="8"/>
-    </row>
-    <row r="81" spans="2:2">
-      <c r="B81" s="8"/>
-    </row>
-    <row r="82" spans="2:2">
-      <c r="B82" s="1"/>
+    <row r="80" spans="2:6">
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="2"/>
+      <c r="E80" t="s">
+        <v>155</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" ht="28" spans="2:6">
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="2"/>
+      <c r="E81" t="s">
+        <v>173</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="82" ht="28" spans="2:6">
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="2"/>
+      <c r="E82" t="s">
+        <v>175</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="83" ht="28" spans="2:6">
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="2"/>
+      <c r="E83" t="s">
+        <v>177</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6">
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="2"/>
+      <c r="E84" t="s">
+        <v>179</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6">
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="2"/>
+      <c r="E85" t="s">
+        <v>180</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E86" t="s">
+        <v>88</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6">
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="2"/>
+      <c r="E87" t="s">
+        <v>186</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6">
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="2"/>
+      <c r="E88" t="s">
+        <v>155</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6">
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="2"/>
+      <c r="E89" t="s">
+        <v>188</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="90" ht="28" spans="2:6">
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="2"/>
+      <c r="E90" t="s">
+        <v>190</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6">
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="2"/>
+      <c r="E91" t="s">
+        <v>192</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6">
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="2"/>
+      <c r="E92" t="s">
+        <v>194</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6">
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="2"/>
+      <c r="E93" t="s">
+        <v>196</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6">
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="2"/>
+      <c r="E94" t="s">
+        <v>198</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6">
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="2"/>
+      <c r="E95" t="s">
+        <v>200</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="96" ht="28" spans="2:6">
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="2"/>
+      <c r="E96" t="s">
+        <v>202</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6">
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="2"/>
+      <c r="E97" t="s">
+        <v>204</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6">
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="2"/>
+      <c r="E98" t="s">
+        <v>206</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6">
+      <c r="B99" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E99" t="s">
+        <v>88</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6">
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="2"/>
+      <c r="E100" t="s">
+        <v>186</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6">
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="2"/>
+      <c r="E101" t="s">
+        <v>210</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6">
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="2"/>
+      <c r="E102" t="s">
+        <v>212</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6">
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="2"/>
+      <c r="E103" t="s">
+        <v>214</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E104" t="s">
+        <v>220</v>
+      </c>
+      <c r="F104" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="105" ht="56" spans="2:6">
+      <c r="B105" s="4"/>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" t="s">
+        <v>222</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E106" t="s">
+        <v>228</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6">
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" t="s">
+        <v>155</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="108" ht="28" spans="2:6">
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" t="s">
+        <v>230</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6">
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" t="s">
+        <v>232</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="110" ht="28" spans="2:6">
+      <c r="B110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4"/>
+      <c r="E110" t="s">
+        <v>234</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6">
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" t="s">
+        <v>236</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" ht="28" spans="2:6">
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" t="s">
+        <v>237</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6">
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" t="s">
+        <v>239</v>
+      </c>
+      <c r="F113" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="114" ht="28" spans="2:6">
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" t="s">
+        <v>241</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="115" ht="28" spans="2:6">
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" t="s">
+        <v>243</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6">
+      <c r="B116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4"/>
+      <c r="E116" t="s">
+        <v>245</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6">
+      <c r="B117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4"/>
+      <c r="E117" t="s">
+        <v>246</v>
+      </c>
+      <c r="F117" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="118" customHeight="1" spans="1:6">
+      <c r="A118" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E118" t="s">
+        <v>220</v>
+      </c>
+      <c r="F118" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6">
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" t="s">
+        <v>253</v>
+      </c>
+      <c r="F119" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6">
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+      <c r="E120" t="s">
+        <v>255</v>
+      </c>
+      <c r="F120" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6">
+      <c r="B121" s="4"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" t="s">
+        <v>257</v>
+      </c>
+      <c r="F121" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6">
+      <c r="B122" s="4"/>
+      <c r="C122" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E122" t="s">
+        <v>220</v>
+      </c>
+      <c r="F122" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6">
+      <c r="B123" s="4"/>
+      <c r="D123" s="4"/>
+      <c r="E123" t="s">
+        <v>261</v>
+      </c>
+      <c r="F123" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6">
+      <c r="B124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" t="s">
+        <v>255</v>
+      </c>
+      <c r="F124" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6">
+      <c r="B125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" t="s">
+        <v>262</v>
+      </c>
+      <c r="F125" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E126" t="s">
+        <v>220</v>
+      </c>
+      <c r="F126" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6">
+      <c r="B127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" t="s">
+        <v>268</v>
+      </c>
+      <c r="F127" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6">
+      <c r="B128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" t="s">
+        <v>269</v>
+      </c>
+      <c r="F128" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6">
+      <c r="B129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" t="s">
+        <v>271</v>
+      </c>
+      <c r="F129" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6">
+      <c r="B130" s="4"/>
+      <c r="D130" s="4"/>
+      <c r="E130" t="s">
+        <v>121</v>
+      </c>
+      <c r="F130" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6">
+      <c r="B131" s="4"/>
+      <c r="D131" s="4"/>
+      <c r="E131" t="s">
+        <v>273</v>
+      </c>
+      <c r="F131" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="132" ht="56" spans="2:6">
+      <c r="B132" s="4"/>
+      <c r="D132" s="4"/>
+      <c r="E132" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6">
+      <c r="B133" s="4"/>
+      <c r="D133" s="4"/>
+      <c r="E133" t="s">
+        <v>106</v>
+      </c>
+      <c r="F133" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6">
+      <c r="B134" s="4"/>
+      <c r="D134" s="4"/>
+      <c r="E134" t="s">
+        <v>277</v>
+      </c>
+      <c r="F134" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E135" t="s">
+        <v>220</v>
+      </c>
+      <c r="F135" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6">
+      <c r="B136" s="4"/>
+      <c r="D136" s="4"/>
+      <c r="E136" t="s">
+        <v>268</v>
+      </c>
+      <c r="F136" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6">
+      <c r="B137" s="4"/>
+      <c r="D137" s="4"/>
+      <c r="E137" t="s">
+        <v>284</v>
+      </c>
+      <c r="F137" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6">
+      <c r="B138" s="4"/>
+      <c r="D138" s="4"/>
+      <c r="E138" t="s">
+        <v>286</v>
+      </c>
+      <c r="F138" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6">
+      <c r="B139" s="4"/>
+      <c r="D139" s="4"/>
+      <c r="E139" t="s">
+        <v>288</v>
+      </c>
+      <c r="F139" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6">
+      <c r="B140" s="4"/>
+      <c r="D140" s="4"/>
+      <c r="E140" t="s">
+        <v>290</v>
+      </c>
+      <c r="F140" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="141" spans="2:6">
+      <c r="B141" s="4"/>
+      <c r="D141" s="4"/>
+      <c r="E141" t="s">
+        <v>292</v>
+      </c>
+      <c r="F141" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="142" ht="28" spans="2:6">
+      <c r="B142" s="4"/>
+      <c r="D142" s="4"/>
+      <c r="E142" t="s">
+        <v>294</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E143" t="s">
+        <v>300</v>
+      </c>
+      <c r="F143" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="144" ht="56" spans="2:6">
+      <c r="B144" s="2"/>
+      <c r="D144" s="2"/>
+      <c r="E144" t="s">
+        <v>302</v>
+      </c>
+      <c r="F144" s="9" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D145" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="E145" t="s">
+        <v>300</v>
+      </c>
+      <c r="F145" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="146" spans="2:6">
+      <c r="B146" s="7"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="7"/>
+      <c r="E146" t="s">
+        <v>308</v>
+      </c>
+      <c r="F146" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6">
+      <c r="B147" s="7"/>
+      <c r="C147" s="2"/>
+      <c r="D147" s="7"/>
+      <c r="E147" t="s">
+        <v>310</v>
+      </c>
+      <c r="F147" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6">
+      <c r="B148" s="7"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="7"/>
+      <c r="E148" t="s">
+        <v>312</v>
+      </c>
+      <c r="F148" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="149" spans="2:6">
+      <c r="B149" s="7"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="7"/>
+      <c r="E149" t="s">
+        <v>314</v>
+      </c>
+      <c r="F149" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="150" spans="2:6">
+      <c r="B150" s="7"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="7"/>
+      <c r="E150" t="s">
+        <v>146</v>
+      </c>
+      <c r="F150" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="151" spans="2:6">
+      <c r="B151" s="7"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="7"/>
+      <c r="E151" t="s">
+        <v>316</v>
+      </c>
+      <c r="F151" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D152" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="E152" t="s">
+        <v>300</v>
+      </c>
+      <c r="F152" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="153" spans="2:6">
+      <c r="B153" s="7"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="7"/>
+      <c r="E153" t="s">
+        <v>322</v>
+      </c>
+      <c r="F153" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="154" spans="2:6">
+      <c r="B154" s="7"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="7"/>
+      <c r="E154" t="s">
+        <v>323</v>
+      </c>
+      <c r="F154" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="155" spans="2:6">
+      <c r="B155" s="7"/>
+      <c r="C155" s="2"/>
+      <c r="D155" s="7"/>
+      <c r="E155" t="s">
+        <v>325</v>
+      </c>
+      <c r="F155" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="156" spans="2:6">
+      <c r="B156" s="7"/>
+      <c r="C156" s="2"/>
+      <c r="D156" s="7"/>
+      <c r="E156" t="s">
+        <v>326</v>
+      </c>
+      <c r="F156" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="D157" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="E157" t="s">
+        <v>332</v>
+      </c>
+      <c r="F157" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="158" spans="2:6">
+      <c r="B158" s="7"/>
+      <c r="C158" s="2"/>
+      <c r="D158" s="8"/>
+      <c r="E158" t="s">
+        <v>334</v>
+      </c>
+      <c r="F158" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="159" ht="56" spans="2:6">
+      <c r="B159" s="7"/>
+      <c r="C159" s="2"/>
+      <c r="D159" s="8"/>
+      <c r="E159" t="s">
+        <v>336</v>
+      </c>
+      <c r="F159" s="9" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B160" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D160" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E160" t="s">
+        <v>332</v>
+      </c>
+      <c r="F160" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="161" spans="2:6">
+      <c r="B161" s="7"/>
+      <c r="C161" s="2"/>
+      <c r="D161" s="8"/>
+      <c r="E161" t="s">
+        <v>334</v>
+      </c>
+      <c r="F161" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="162" spans="2:6">
+      <c r="B162" s="7"/>
+      <c r="C162" s="2"/>
+      <c r="D162" s="8"/>
+      <c r="E162" t="s">
+        <v>342</v>
+      </c>
+      <c r="F162" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="163" ht="28" spans="2:6">
+      <c r="B163" s="7"/>
+      <c r="C163" s="2"/>
+      <c r="D163" s="8"/>
+      <c r="E163" t="s">
+        <v>344</v>
+      </c>
+      <c r="F163" s="9" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="164" spans="2:6">
+      <c r="B164" s="7"/>
+      <c r="C164" s="2"/>
+      <c r="D164" s="8"/>
+      <c r="E164" t="s">
+        <v>346</v>
+      </c>
+      <c r="F164" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="165" spans="2:6">
+      <c r="B165" s="7"/>
+      <c r="C165" s="2"/>
+      <c r="D165" s="8"/>
+      <c r="E165" t="s">
+        <v>348</v>
+      </c>
+      <c r="F165" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="166" spans="2:6">
+      <c r="B166" s="7"/>
+      <c r="C166" s="2"/>
+      <c r="D166" s="8"/>
+      <c r="E166" t="s">
+        <v>350</v>
+      </c>
+      <c r="F166" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="167" spans="2:6">
+      <c r="B167" s="7"/>
+      <c r="C167" s="2"/>
+      <c r="D167" s="8"/>
+      <c r="E167" t="s">
+        <v>352</v>
+      </c>
+      <c r="F167" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="168" spans="2:6">
+      <c r="B168" s="7"/>
+      <c r="C168" s="2"/>
+      <c r="D168" s="8"/>
+      <c r="E168" t="s">
+        <v>354</v>
+      </c>
+      <c r="F168" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="E169" t="s">
+        <v>332</v>
+      </c>
+      <c r="F169" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="170" spans="2:6">
+      <c r="B170" s="7"/>
+      <c r="C170" s="4"/>
+      <c r="D170" s="7"/>
+      <c r="E170" t="s">
+        <v>334</v>
+      </c>
+      <c r="F170" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="171" spans="2:6">
+      <c r="B171" s="7"/>
+      <c r="C171" s="4"/>
+      <c r="D171" s="7"/>
+      <c r="E171" t="s">
+        <v>362</v>
+      </c>
+      <c r="F171" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="172" spans="2:6">
+      <c r="B172" s="7"/>
+      <c r="C172" s="4"/>
+      <c r="D172" s="7"/>
+      <c r="E172" t="s">
+        <v>364</v>
+      </c>
+      <c r="F172" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="173" spans="2:6">
+      <c r="B173" s="7"/>
+      <c r="C173" s="4"/>
+      <c r="D173" s="7"/>
+      <c r="E173" t="s">
+        <v>350</v>
+      </c>
+      <c r="F173" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="174" ht="28" spans="2:6">
+      <c r="B174" s="7"/>
+      <c r="C174" s="4"/>
+      <c r="D174" s="7"/>
+      <c r="E174" t="s">
+        <v>366</v>
+      </c>
+      <c r="F174" s="9" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="175" ht="28" spans="2:6">
+      <c r="B175" s="7"/>
+      <c r="C175" s="4"/>
+      <c r="D175" s="7"/>
+      <c r="E175" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="F175" s="9" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="176" spans="2:6">
+      <c r="B176" s="7"/>
+      <c r="C176" s="4"/>
+      <c r="D176" s="7"/>
+      <c r="E176" t="s">
+        <v>255</v>
+      </c>
+      <c r="F176" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="177" spans="2:6">
+      <c r="B177" s="7"/>
+      <c r="C177" s="4"/>
+      <c r="D177" s="7"/>
+      <c r="E177" t="s">
+        <v>371</v>
+      </c>
+      <c r="F177" t="s">
+        <v>372</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="89">
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="A13:A33"/>
     <mergeCell ref="A37:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A69"/>
-    <mergeCell ref="A70:A77"/>
+    <mergeCell ref="A56:A67"/>
+    <mergeCell ref="A68:A76"/>
+    <mergeCell ref="A77:A85"/>
+    <mergeCell ref="A86:A98"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="A106:A117"/>
+    <mergeCell ref="A118:A125"/>
+    <mergeCell ref="A126:A134"/>
+    <mergeCell ref="A135:A142"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="A145:A151"/>
+    <mergeCell ref="A152:A156"/>
+    <mergeCell ref="A157:A159"/>
+    <mergeCell ref="A160:A168"/>
+    <mergeCell ref="A169:A177"/>
     <mergeCell ref="B2:B12"/>
     <mergeCell ref="B13:B33"/>
     <mergeCell ref="B37:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B69"/>
-    <mergeCell ref="B70:B77"/>
+    <mergeCell ref="B56:B67"/>
+    <mergeCell ref="B68:B76"/>
+    <mergeCell ref="B77:B85"/>
+    <mergeCell ref="B86:B98"/>
+    <mergeCell ref="B99:B103"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="B106:B117"/>
+    <mergeCell ref="B118:B125"/>
+    <mergeCell ref="B126:B134"/>
+    <mergeCell ref="B135:B142"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="B145:B151"/>
+    <mergeCell ref="B152:B156"/>
+    <mergeCell ref="B157:B159"/>
+    <mergeCell ref="B160:B168"/>
+    <mergeCell ref="B169:B177"/>
     <mergeCell ref="C2:C8"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="C13:C16"/>
@@ -2646,10 +4456,23 @@
     <mergeCell ref="C27:C29"/>
     <mergeCell ref="C30:C33"/>
     <mergeCell ref="C37:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C58:C69"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C74:C77"/>
+    <mergeCell ref="C56:C67"/>
+    <mergeCell ref="C68:C76"/>
+    <mergeCell ref="C77:C85"/>
+    <mergeCell ref="C86:C98"/>
+    <mergeCell ref="C99:C103"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="C106:C117"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="C122:C125"/>
+    <mergeCell ref="C126:C134"/>
+    <mergeCell ref="C135:C142"/>
+    <mergeCell ref="C143:C144"/>
+    <mergeCell ref="C145:C151"/>
+    <mergeCell ref="C152:C156"/>
+    <mergeCell ref="C157:C159"/>
+    <mergeCell ref="C160:C168"/>
+    <mergeCell ref="C169:C177"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="D9:D12"/>
     <mergeCell ref="D13:D16"/>
@@ -2659,10 +4482,23 @@
     <mergeCell ref="D27:D29"/>
     <mergeCell ref="D30:D33"/>
     <mergeCell ref="D37:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D58:D69"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="D74:D77"/>
+    <mergeCell ref="D56:D67"/>
+    <mergeCell ref="D68:D76"/>
+    <mergeCell ref="D77:D85"/>
+    <mergeCell ref="D86:D98"/>
+    <mergeCell ref="D99:D103"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="D106:D117"/>
+    <mergeCell ref="D118:D121"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="D126:D134"/>
+    <mergeCell ref="D135:D142"/>
+    <mergeCell ref="D143:D144"/>
+    <mergeCell ref="D145:D151"/>
+    <mergeCell ref="D152:D156"/>
+    <mergeCell ref="D157:D159"/>
+    <mergeCell ref="D160:D168"/>
+    <mergeCell ref="D169:D177"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Time page validation test done
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/data/Source_File.xlsx
+++ b/src/main/java/org/example/data/Source_File.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11760" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382">
   <si>
     <t>Firstname</t>
   </si>
@@ -1164,16 +1164,43 @@
   <si>
     <t xml:space="preserve">User should see a leave list display on the page </t>
   </si>
+  <si>
+    <t>S22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time page validation </t>
+  </si>
+  <si>
+    <t>User should be able to see all the links on the time page</t>
+  </si>
+  <si>
+    <t>Navigate to the "Time" page</t>
+  </si>
+  <si>
+    <t>User should see time page</t>
+  </si>
+  <si>
+    <t>Click On "Time" link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be able to click time link </t>
+  </si>
+  <si>
+    <t>Verify all the links display on the page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see following links display on the page: TimeSheets, Attendance, Reports, Project Info. My Timesheets, Employee timesheets, My Records, Punch In/Out, Employee Records, Confuguration, Project Reports, Employee Repoerts, Attendance Summary, Customers, Projects. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1200,10 +1227,57 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1222,8 +1296,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1237,33 +1312,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1277,37 +1335,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1321,14 +1349,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -1336,11 +1356,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1354,6 +1381,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1377,6 +1422,132 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1389,157 +1560,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1550,6 +1577,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1564,35 +1624,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1614,8 +1645,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1636,17 +1669,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1655,145 +1682,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1823,10 +1850,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2202,10 +2229,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G177"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="E177" sqref="E177"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
@@ -3996,7 +4023,7 @@
       <c r="E144" t="s">
         <v>302</v>
       </c>
-      <c r="F144" s="9" t="s">
+      <c r="F144" s="1" t="s">
         <v>303</v>
       </c>
     </row>
@@ -4004,13 +4031,13 @@
       <c r="A145" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B145" s="7" t="s">
+      <c r="B145" s="4" t="s">
         <v>305</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D145" s="7" t="s">
+      <c r="D145" s="4" t="s">
         <v>307</v>
       </c>
       <c r="E145" t="s">
@@ -4021,9 +4048,8 @@
       </c>
     </row>
     <row r="146" spans="2:6">
-      <c r="B146" s="7"/>
-      <c r="C146" s="2"/>
-      <c r="D146" s="7"/>
+      <c r="B146" s="4"/>
+      <c r="D146" s="4"/>
       <c r="E146" t="s">
         <v>308</v>
       </c>
@@ -4032,9 +4058,8 @@
       </c>
     </row>
     <row r="147" spans="2:6">
-      <c r="B147" s="7"/>
-      <c r="C147" s="2"/>
-      <c r="D147" s="7"/>
+      <c r="B147" s="4"/>
+      <c r="D147" s="4"/>
       <c r="E147" t="s">
         <v>310</v>
       </c>
@@ -4043,9 +4068,8 @@
       </c>
     </row>
     <row r="148" spans="2:6">
-      <c r="B148" s="7"/>
-      <c r="C148" s="2"/>
-      <c r="D148" s="7"/>
+      <c r="B148" s="4"/>
+      <c r="D148" s="4"/>
       <c r="E148" t="s">
         <v>312</v>
       </c>
@@ -4054,9 +4078,8 @@
       </c>
     </row>
     <row r="149" spans="2:6">
-      <c r="B149" s="7"/>
-      <c r="C149" s="2"/>
-      <c r="D149" s="7"/>
+      <c r="B149" s="4"/>
+      <c r="D149" s="4"/>
       <c r="E149" t="s">
         <v>314</v>
       </c>
@@ -4065,9 +4088,8 @@
       </c>
     </row>
     <row r="150" spans="2:6">
-      <c r="B150" s="7"/>
-      <c r="C150" s="2"/>
-      <c r="D150" s="7"/>
+      <c r="B150" s="4"/>
+      <c r="D150" s="4"/>
       <c r="E150" t="s">
         <v>146</v>
       </c>
@@ -4076,9 +4098,8 @@
       </c>
     </row>
     <row r="151" spans="2:6">
-      <c r="B151" s="7"/>
-      <c r="C151" s="2"/>
-      <c r="D151" s="7"/>
+      <c r="B151" s="4"/>
+      <c r="D151" s="4"/>
       <c r="E151" t="s">
         <v>316</v>
       </c>
@@ -4090,13 +4111,13 @@
       <c r="A152" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B152" s="7" t="s">
+      <c r="B152" s="4" t="s">
         <v>319</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D152" s="7" t="s">
+      <c r="D152" s="4" t="s">
         <v>321</v>
       </c>
       <c r="E152" t="s">
@@ -4107,9 +4128,8 @@
       </c>
     </row>
     <row r="153" spans="2:6">
-      <c r="B153" s="7"/>
-      <c r="C153" s="2"/>
-      <c r="D153" s="7"/>
+      <c r="B153" s="4"/>
+      <c r="D153" s="4"/>
       <c r="E153" t="s">
         <v>322</v>
       </c>
@@ -4118,9 +4138,8 @@
       </c>
     </row>
     <row r="154" spans="2:6">
-      <c r="B154" s="7"/>
-      <c r="C154" s="2"/>
-      <c r="D154" s="7"/>
+      <c r="B154" s="4"/>
+      <c r="D154" s="4"/>
       <c r="E154" t="s">
         <v>323</v>
       </c>
@@ -4129,9 +4148,8 @@
       </c>
     </row>
     <row r="155" spans="2:6">
-      <c r="B155" s="7"/>
-      <c r="C155" s="2"/>
-      <c r="D155" s="7"/>
+      <c r="B155" s="4"/>
+      <c r="D155" s="4"/>
       <c r="E155" t="s">
         <v>325</v>
       </c>
@@ -4140,9 +4158,8 @@
       </c>
     </row>
     <row r="156" spans="2:6">
-      <c r="B156" s="7"/>
-      <c r="C156" s="2"/>
-      <c r="D156" s="7"/>
+      <c r="B156" s="4"/>
+      <c r="D156" s="4"/>
       <c r="E156" t="s">
         <v>326</v>
       </c>
@@ -4154,13 +4171,13 @@
       <c r="A157" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B157" s="7" t="s">
+      <c r="B157" s="4" t="s">
         <v>329</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="D157" s="7" t="s">
+      <c r="D157" s="4" t="s">
         <v>331</v>
       </c>
       <c r="E157" t="s">
@@ -4171,9 +4188,8 @@
       </c>
     </row>
     <row r="158" spans="2:6">
-      <c r="B158" s="7"/>
-      <c r="C158" s="2"/>
-      <c r="D158" s="8"/>
+      <c r="B158" s="4"/>
+      <c r="D158" s="2"/>
       <c r="E158" t="s">
         <v>334</v>
       </c>
@@ -4182,13 +4198,12 @@
       </c>
     </row>
     <row r="159" ht="56" spans="2:6">
-      <c r="B159" s="7"/>
-      <c r="C159" s="2"/>
-      <c r="D159" s="8"/>
+      <c r="B159" s="4"/>
+      <c r="D159" s="2"/>
       <c r="E159" t="s">
         <v>336</v>
       </c>
-      <c r="F159" s="9" t="s">
+      <c r="F159" s="1" t="s">
         <v>337</v>
       </c>
     </row>
@@ -4196,13 +4211,13 @@
       <c r="A160" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B160" s="7" t="s">
+      <c r="B160" s="4" t="s">
         <v>339</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="D160" s="8" t="s">
+      <c r="D160" s="2" t="s">
         <v>341</v>
       </c>
       <c r="E160" t="s">
@@ -4213,9 +4228,8 @@
       </c>
     </row>
     <row r="161" spans="2:6">
-      <c r="B161" s="7"/>
-      <c r="C161" s="2"/>
-      <c r="D161" s="8"/>
+      <c r="B161" s="4"/>
+      <c r="D161" s="2"/>
       <c r="E161" t="s">
         <v>334</v>
       </c>
@@ -4224,9 +4238,8 @@
       </c>
     </row>
     <row r="162" spans="2:6">
-      <c r="B162" s="7"/>
-      <c r="C162" s="2"/>
-      <c r="D162" s="8"/>
+      <c r="B162" s="4"/>
+      <c r="D162" s="2"/>
       <c r="E162" t="s">
         <v>342</v>
       </c>
@@ -4235,20 +4248,18 @@
       </c>
     </row>
     <row r="163" ht="28" spans="2:6">
-      <c r="B163" s="7"/>
-      <c r="C163" s="2"/>
-      <c r="D163" s="8"/>
+      <c r="B163" s="4"/>
+      <c r="D163" s="2"/>
       <c r="E163" t="s">
         <v>344</v>
       </c>
-      <c r="F163" s="9" t="s">
+      <c r="F163" s="1" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="164" spans="2:6">
-      <c r="B164" s="7"/>
-      <c r="C164" s="2"/>
-      <c r="D164" s="8"/>
+      <c r="B164" s="4"/>
+      <c r="D164" s="2"/>
       <c r="E164" t="s">
         <v>346</v>
       </c>
@@ -4257,9 +4268,8 @@
       </c>
     </row>
     <row r="165" spans="2:6">
-      <c r="B165" s="7"/>
-      <c r="C165" s="2"/>
-      <c r="D165" s="8"/>
+      <c r="B165" s="4"/>
+      <c r="D165" s="2"/>
       <c r="E165" t="s">
         <v>348</v>
       </c>
@@ -4268,9 +4278,8 @@
       </c>
     </row>
     <row r="166" spans="2:6">
-      <c r="B166" s="7"/>
-      <c r="C166" s="2"/>
-      <c r="D166" s="8"/>
+      <c r="B166" s="4"/>
+      <c r="D166" s="2"/>
       <c r="E166" t="s">
         <v>350</v>
       </c>
@@ -4279,9 +4288,8 @@
       </c>
     </row>
     <row r="167" spans="2:6">
-      <c r="B167" s="7"/>
-      <c r="C167" s="2"/>
-      <c r="D167" s="8"/>
+      <c r="B167" s="4"/>
+      <c r="D167" s="2"/>
       <c r="E167" t="s">
         <v>352</v>
       </c>
@@ -4290,9 +4298,8 @@
       </c>
     </row>
     <row r="168" spans="2:6">
-      <c r="B168" s="7"/>
-      <c r="C168" s="2"/>
-      <c r="D168" s="8"/>
+      <c r="B168" s="4"/>
+      <c r="D168" s="2"/>
       <c r="E168" t="s">
         <v>354</v>
       </c>
@@ -4304,13 +4311,13 @@
       <c r="A169" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="B169" s="7" t="s">
+      <c r="B169" s="4" t="s">
         <v>357</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="D169" s="7" t="s">
+      <c r="D169" s="4" t="s">
         <v>359</v>
       </c>
       <c r="E169" t="s">
@@ -4321,9 +4328,9 @@
       </c>
     </row>
     <row r="170" spans="2:6">
-      <c r="B170" s="7"/>
+      <c r="B170" s="4"/>
       <c r="C170" s="4"/>
-      <c r="D170" s="7"/>
+      <c r="D170" s="4"/>
       <c r="E170" t="s">
         <v>334</v>
       </c>
@@ -4332,9 +4339,9 @@
       </c>
     </row>
     <row r="171" spans="2:6">
-      <c r="B171" s="7"/>
+      <c r="B171" s="4"/>
       <c r="C171" s="4"/>
-      <c r="D171" s="7"/>
+      <c r="D171" s="4"/>
       <c r="E171" t="s">
         <v>362</v>
       </c>
@@ -4343,9 +4350,9 @@
       </c>
     </row>
     <row r="172" spans="2:6">
-      <c r="B172" s="7"/>
+      <c r="B172" s="4"/>
       <c r="C172" s="4"/>
-      <c r="D172" s="7"/>
+      <c r="D172" s="4"/>
       <c r="E172" t="s">
         <v>364</v>
       </c>
@@ -4354,9 +4361,9 @@
       </c>
     </row>
     <row r="173" spans="2:6">
-      <c r="B173" s="7"/>
+      <c r="B173" s="4"/>
       <c r="C173" s="4"/>
-      <c r="D173" s="7"/>
+      <c r="D173" s="4"/>
       <c r="E173" t="s">
         <v>350</v>
       </c>
@@ -4365,31 +4372,31 @@
       </c>
     </row>
     <row r="174" ht="28" spans="2:6">
-      <c r="B174" s="7"/>
+      <c r="B174" s="4"/>
       <c r="C174" s="4"/>
-      <c r="D174" s="7"/>
+      <c r="D174" s="4"/>
       <c r="E174" t="s">
         <v>366</v>
       </c>
-      <c r="F174" s="9" t="s">
+      <c r="F174" s="1" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="175" ht="28" spans="2:6">
-      <c r="B175" s="7"/>
+      <c r="B175" s="4"/>
       <c r="C175" s="4"/>
-      <c r="D175" s="7"/>
-      <c r="E175" s="9" t="s">
+      <c r="D175" s="4"/>
+      <c r="E175" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="F175" s="9" t="s">
+      <c r="F175" s="1" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="176" spans="2:6">
-      <c r="B176" s="7"/>
+      <c r="B176" s="4"/>
       <c r="C176" s="4"/>
-      <c r="D176" s="7"/>
+      <c r="D176" s="4"/>
       <c r="E176" t="s">
         <v>255</v>
       </c>
@@ -4398,9 +4405,9 @@
       </c>
     </row>
     <row r="177" spans="2:6">
-      <c r="B177" s="7"/>
+      <c r="B177" s="4"/>
       <c r="C177" s="4"/>
-      <c r="D177" s="7"/>
+      <c r="D177" s="4"/>
       <c r="E177" t="s">
         <v>371</v>
       </c>
@@ -4408,8 +4415,50 @@
         <v>372</v>
       </c>
     </row>
+    <row r="178" spans="1:6">
+      <c r="A178" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D178" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="E178" t="s">
+        <v>376</v>
+      </c>
+      <c r="F178" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="179" spans="2:6">
+      <c r="B179" s="7"/>
+      <c r="C179" s="2"/>
+      <c r="D179" s="8"/>
+      <c r="E179" t="s">
+        <v>378</v>
+      </c>
+      <c r="F179" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="180" ht="98" spans="2:6">
+      <c r="B180" s="7"/>
+      <c r="C180" s="2"/>
+      <c r="D180" s="8"/>
+      <c r="E180" t="s">
+        <v>380</v>
+      </c>
+      <c r="F180" s="9" t="s">
+        <v>381</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="89">
+  <mergeCells count="93">
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="A13:A33"/>
     <mergeCell ref="A37:A55"/>
@@ -4428,6 +4477,7 @@
     <mergeCell ref="A157:A159"/>
     <mergeCell ref="A160:A168"/>
     <mergeCell ref="A169:A177"/>
+    <mergeCell ref="A178:A180"/>
     <mergeCell ref="B2:B12"/>
     <mergeCell ref="B13:B33"/>
     <mergeCell ref="B37:B55"/>
@@ -4447,6 +4497,7 @@
     <mergeCell ref="B157:B159"/>
     <mergeCell ref="B160:B168"/>
     <mergeCell ref="B169:B177"/>
+    <mergeCell ref="B178:B180"/>
     <mergeCell ref="C2:C8"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="C13:C16"/>
@@ -4473,6 +4524,7 @@
     <mergeCell ref="C157:C159"/>
     <mergeCell ref="C160:C168"/>
     <mergeCell ref="C169:C177"/>
+    <mergeCell ref="C178:C180"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="D9:D12"/>
     <mergeCell ref="D13:D16"/>
@@ -4499,6 +4551,7 @@
     <mergeCell ref="D157:D159"/>
     <mergeCell ref="D160:D168"/>
     <mergeCell ref="D169:D177"/>
+    <mergeCell ref="D178:D180"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>